<commit_message>
Link Bieu Mau to Tien Ich + View online
</commit_message>
<xml_diff>
--- a/file_export/bieu_mau/Mau m2.xlsx
+++ b/file_export/bieu_mau/Mau m2.xlsx
@@ -139,6 +139,24 @@
     </font>
     <font>
       <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="single"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -170,24 +188,6 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -272,58 +272,58 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -628,44 +628,44 @@
   <dimension ref="A1:AG10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="true" style="3"/>
-    <col min="2" max="2" width="5.140625" customWidth="true" style="3"/>
-    <col min="3" max="3" width="5.140625" customWidth="true" style="3"/>
-    <col min="4" max="4" width="5.140625" customWidth="true" style="3"/>
-    <col min="5" max="5" width="5.140625" customWidth="true" style="3"/>
-    <col min="6" max="6" width="5.140625" customWidth="true" style="3"/>
-    <col min="7" max="7" width="5.140625" customWidth="true" style="3"/>
-    <col min="8" max="8" width="5.140625" customWidth="true" style="3"/>
-    <col min="9" max="9" width="5.140625" customWidth="true" style="3"/>
-    <col min="10" max="10" width="5.140625" customWidth="true" style="3"/>
-    <col min="11" max="11" width="5.140625" customWidth="true" style="3"/>
-    <col min="12" max="12" width="5.140625" customWidth="true" style="3"/>
-    <col min="13" max="13" width="5.140625" customWidth="true" style="3"/>
-    <col min="14" max="14" width="5.140625" customWidth="true" style="3"/>
-    <col min="15" max="15" width="5.140625" customWidth="true" style="3"/>
-    <col min="16" max="16" width="5.140625" customWidth="true" style="3"/>
-    <col min="17" max="17" width="5.140625" customWidth="true" style="3"/>
-    <col min="18" max="18" width="5.140625" customWidth="true" style="3"/>
-    <col min="19" max="19" width="5.140625" customWidth="true" style="3"/>
-    <col min="20" max="20" width="5.140625" customWidth="true" style="3"/>
-    <col min="21" max="21" width="5.140625" customWidth="true" style="3"/>
-    <col min="22" max="22" width="5.140625" customWidth="true" style="3"/>
-    <col min="23" max="23" width="5.140625" customWidth="true" style="3"/>
-    <col min="24" max="24" width="5.140625" customWidth="true" style="3"/>
-    <col min="25" max="25" width="5.140625" customWidth="true" style="3"/>
-    <col min="26" max="26" width="5.140625" customWidth="true" style="3"/>
-    <col min="27" max="27" width="5.140625" customWidth="true" style="3"/>
-    <col min="28" max="28" width="5.140625" customWidth="true" style="3"/>
-    <col min="29" max="29" width="5.140625" customWidth="true" style="3"/>
-    <col min="30" max="30" width="5.140625" customWidth="true" style="3"/>
-    <col min="31" max="31" width="5.140625" customWidth="true" style="3"/>
-    <col min="32" max="32" width="5.140625" customWidth="true" style="3"/>
-    <col min="33" max="33" width="9.140625" customWidth="true" style="3"/>
+    <col min="1" max="1" width="5.140625" customWidth="true" style="2"/>
+    <col min="2" max="2" width="5.140625" customWidth="true" style="2"/>
+    <col min="3" max="3" width="5.140625" customWidth="true" style="2"/>
+    <col min="4" max="4" width="5.140625" customWidth="true" style="2"/>
+    <col min="5" max="5" width="5.140625" customWidth="true" style="2"/>
+    <col min="6" max="6" width="5.140625" customWidth="true" style="2"/>
+    <col min="7" max="7" width="5.140625" customWidth="true" style="2"/>
+    <col min="8" max="8" width="5.140625" customWidth="true" style="2"/>
+    <col min="9" max="9" width="5.140625" customWidth="true" style="2"/>
+    <col min="10" max="10" width="5.140625" customWidth="true" style="2"/>
+    <col min="11" max="11" width="5.140625" customWidth="true" style="2"/>
+    <col min="12" max="12" width="5.140625" customWidth="true" style="2"/>
+    <col min="13" max="13" width="5.140625" customWidth="true" style="2"/>
+    <col min="14" max="14" width="5.140625" customWidth="true" style="2"/>
+    <col min="15" max="15" width="5.140625" customWidth="true" style="2"/>
+    <col min="16" max="16" width="5.140625" customWidth="true" style="2"/>
+    <col min="17" max="17" width="5.140625" customWidth="true" style="2"/>
+    <col min="18" max="18" width="5.140625" customWidth="true" style="2"/>
+    <col min="19" max="19" width="5.140625" customWidth="true" style="2"/>
+    <col min="20" max="20" width="5.140625" customWidth="true" style="2"/>
+    <col min="21" max="21" width="5.140625" customWidth="true" style="2"/>
+    <col min="22" max="22" width="5.140625" customWidth="true" style="2"/>
+    <col min="23" max="23" width="5.140625" customWidth="true" style="2"/>
+    <col min="24" max="24" width="5.140625" customWidth="true" style="2"/>
+    <col min="25" max="25" width="5.140625" customWidth="true" style="2"/>
+    <col min="26" max="26" width="5.140625" customWidth="true" style="2"/>
+    <col min="27" max="27" width="5.140625" customWidth="true" style="2"/>
+    <col min="28" max="28" width="5.140625" customWidth="true" style="2"/>
+    <col min="29" max="29" width="5.140625" customWidth="true" style="2"/>
+    <col min="30" max="30" width="5.140625" customWidth="true" style="2"/>
+    <col min="31" max="31" width="5.140625" customWidth="true" style="2"/>
+    <col min="32" max="32" width="5.140625" customWidth="true" style="2"/>
+    <col min="33" max="33" width="9.140625" customWidth="true" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -696,87 +696,87 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
     <row r="2" spans="1:33" customHeight="1" ht="15.75">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
     </row>
     <row r="3" spans="1:33" customHeight="1" ht="15.75">
       <c r="A3" s="1"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="1"/>
@@ -789,13 +789,13 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -808,42 +808,42 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
     </row>
     <row r="5" spans="1:33" customHeight="1" ht="15.75">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
@@ -883,280 +883,291 @@
       <c r="AF6" s="1"/>
     </row>
     <row r="7" spans="1:33">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="9" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
     </row>
     <row r="8" spans="1:33" customHeight="1" ht="33.75">
-      <c r="A8" s="9"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13" t="s">
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14" t="s">
+      <c r="L8" s="15"/>
+      <c r="M8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="14"/>
-      <c r="O8" s="15" t="s">
+      <c r="N8" s="10"/>
+      <c r="O8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="13" t="s">
+      <c r="P8" s="17"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="S8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="T8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13" t="s">
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13" t="s">
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="14" t="s">
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="15" t="s">
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="17"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="18"/>
     </row>
     <row r="9" spans="1:33" customHeight="1" ht="99">
-      <c r="A9" s="9"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="18" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="20" t="s">
+      <c r="O9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="Q9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="18" t="s">
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="U9" s="18" t="s">
+      <c r="U9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="18" t="s">
+      <c r="V9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W9" s="19" t="s">
+      <c r="W9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X9" s="19" t="s">
+      <c r="X9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y9" s="19" t="s">
+      <c r="Y9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z9" s="18" t="s">
+      <c r="Z9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA9" s="18" t="s">
+      <c r="AA9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB9" s="19" t="s">
+      <c r="AB9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC9" s="19" t="s">
+      <c r="AC9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AD9" s="20" t="s">
+      <c r="AD9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE9" s="19" t="s">
+      <c r="AE9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF9" s="19" t="s">
+      <c r="AF9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:33">
-      <c r="A10" s="21">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22">
+      <c r="C10" s="8"/>
+      <c r="D10" s="9">
         <v>21</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="9">
         <v>68</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="9">
         <v>45</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="9">
         <v>1</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22">
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
         <v>2</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="9">
         <v>2</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21">
+      <c r="K10" s="9"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8">
         <v>1</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="8">
         <v>1</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="8">
         <v>0</v>
       </c>
-      <c r="P10" s="21">
+      <c r="P10" s="8">
         <v>0</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="8">
         <v>2</v>
       </c>
-      <c r="R10" s="21">
+      <c r="R10" s="8">
         <v>2</v>
       </c>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21">
+      <c r="S10" s="8"/>
+      <c r="T10" s="8">
         <v>21</v>
       </c>
-      <c r="U10" s="21">
+      <c r="U10" s="8">
         <v>21</v>
       </c>
-      <c r="V10" s="21">
+      <c r="V10" s="8">
         <v>21</v>
       </c>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21">
+      <c r="W10" s="8">
+        <v>0</v>
+      </c>
+      <c r="X10" s="8">
         <v>2</v>
       </c>
-      <c r="Y10" s="21">
+      <c r="Y10" s="8">
         <v>2</v>
       </c>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21">
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8">
         <v>0</v>
       </c>
-      <c r="AC10" s="21">
+      <c r="AC10" s="8">
         <v>2</v>
       </c>
-      <c r="AD10" s="21">
+      <c r="AD10" s="8">
         <v>0</v>
       </c>
-      <c r="AE10" s="21">
+      <c r="AE10" s="8">
         <v>0</v>
       </c>
-      <c r="AF10" s="21">
+      <c r="AF10" s="8">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="A5:AC5"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="U2:AF2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="U3:AF3"/>
     <mergeCell ref="AB8:AC8"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:Q7"/>
@@ -1173,13 +1184,6 @@
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="T8:V8"/>
     <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="A5:AC5"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="U2:AF2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="U3:AF3"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>